<commit_message>
Update Negative Jump Detailed Cases.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Negative Jump Detailed Cases.xlsx
+++ b/Documents/Negative Jump Detailed Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jay\Documents\Ultimate Datetime Datatype\Ultimate Datetime\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1146268-6F74-4410-A513-32758D5F993D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8207D5A9-4F45-4B64-BDBA-881CC07C6B1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{D614729A-84EA-41FF-B897-0E3AB60D6923}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t>Cases</t>
   </si>
@@ -270,7 +270,7 @@
     <t>C - In Other Ambiguous Region</t>
   </si>
   <si>
-    <t>N / A</t>
+    <t>Use post jump value of UTC2</t>
   </si>
   <si>
     <t>Subtract .05 from TAI1 + RTAI and use pre jump value of UTC2</t>
@@ -307,6 +307,21 @@
   </si>
   <si>
     <t>****** Need to do UTC1 - RTAI</t>
+  </si>
+  <si>
+    <t>TAI1 - RTAI / UTC1</t>
+  </si>
+  <si>
+    <t>Use post Jump value of UTC2 (since UTC1 had to be after ambiguous regions)</t>
+  </si>
+  <si>
+    <t>Make a positive adjustment to TAI1 - RTAI</t>
+  </si>
+  <si>
+    <t>Add .10 to TAI1 - RTAI and use post jump value of UTC2</t>
+  </si>
+  <si>
+    <t>Handled by C-A</t>
   </si>
 </sst>
 </file>
@@ -683,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD82806-C0BC-4AE4-B821-A10DE4446123}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1171,7 +1186,7 @@
         <v>90</v>
       </c>
       <c r="D70" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.75">
@@ -1230,7 +1245,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -1238,10 +1253,69 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A82" t="s">
         <v>82</v>
       </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A85" t="s">
+        <v>64</v>
+      </c>
+      <c r="B85" t="s">
+        <v>66</v>
+      </c>
+      <c r="C85" t="s">
+        <v>67</v>
+      </c>
+      <c r="D85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A86" t="s">
+        <v>65</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A87" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="B88" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>